<commit_message>
sintaxe do for loop corrigido
</commit_message>
<xml_diff>
--- a/Planilha de Compras v2.xlsx
+++ b/Planilha de Compras v2.xlsx
@@ -2,26 +2,34 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <workbookProtection/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Frutas" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Cores" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="2">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <b val="1"/>
       <color theme="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
@@ -35,7 +43,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -43,15 +51,39 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -434,94 +466,184 @@
   </sheetPr>
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="9.140625" customWidth="1" style="1" min="1" max="1"/>
+    <col width="11.85546875" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
+    <col width="12.42578125" customWidth="1" style="1" min="3" max="3"/>
+    <col width="9.140625" customWidth="1" style="1" min="4" max="16384"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
         <is>
           <t>Fruta</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t xml:space="preserve"> Quantidade</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>Preço</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>Banana</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> 9</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>0,99</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>Maça</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> 7</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="2" t="inlineStr">
         <is>
           <t>9,00</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>Pera</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve"> 11</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
+      <c r="C4" s="2" t="inlineStr">
         <is>
           <t>1,00</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Uva</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Fruta 1</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
         <is>
           <t>3</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
+      <c r="C5" s="2" t="inlineStr">
         <is>
           <t>0,50</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="9.140625" customWidth="1" style="1" min="1" max="1"/>
+    <col width="10.7109375" bestFit="1" customWidth="1" style="1" min="2" max="2"/>
+    <col width="9.140625" customWidth="1" style="1" min="3" max="16384"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Primária</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>Secundária</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Azul</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>Amarelo</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Verde</t>
+        </is>
+      </c>
+      <c r="B3" s="2" t="inlineStr">
+        <is>
+          <t>Vermelho</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Rosa</t>
+        </is>
+      </c>
+      <c r="B4" s="2" t="inlineStr">
+        <is>
+          <t>Preto</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Branco</t>
+        </is>
+      </c>
+      <c r="B5" s="2" t="inlineStr">
+        <is>
+          <t>Laranja</t>
         </is>
       </c>
     </row>

</xml_diff>